<commit_message>
Atualização no plano de aulas.
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Data</t>
   </si>
@@ -98,7 +98,25 @@
     <t xml:space="preserve">Expositiva; Atividade prática: reforma de um projeto que apresenta más práticas de projeto</t>
   </si>
   <si>
+    <t xml:space="preserve">Distribuição e versionamento de software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferramentas de distribuição de software. Tipos de distribuição. Esquemas de versionamento. Referência: FOGEL Cap 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expositiva; Atividade prática: criação de um pacote Python para distribuição via pip e de um pacote Debian para instalação em sistemas baseados em Debian.</t>
+  </si>
+  <si>
     <t>FERIADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como fazer software funcionar em vários países?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definição de localização e internacionalização. Ferramenta gettext para traduções e format .po.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expositiva; Atividade prática: tradução e localização de um aplicativo linha de comando e de um sistema web em Flask.</t>
   </si>
   <si>
     <t xml:space="preserve">Testes de software</t>
@@ -111,22 +129,7 @@
 Prática: adiciona testes de unidade e de interface ao projeto da atividade passada</t>
   </si>
   <si>
-    <t xml:space="preserve">Distribuição e versionamento de software</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferramentas de distribuição de software. Tipos de distribuição. Esquemas de versionamento. Referência: FOGEL Cap 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expositiva; Atividade prática: criação de um pacote Python para distribuição via pip e de um pacote Debian para instalação em sistemas baseados em Debian.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como fazer software funcionar em vários países?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definição de localização e internacionalização. Ferramenta gettext para traduções e format .po.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expositiva; Atividade prática: tradução e localização de um aplicativo linha de comando e de um sistema web em Flask.</t>
+    <t xml:space="preserve">Aula estúdio para atividade “Testes de Software” </t>
   </si>
   <si>
     <t xml:space="preserve">Licenças de software</t>
@@ -139,13 +142,13 @@
     <t xml:space="preserve">Expositiva; Atividade prática: discussões de casos relevantes recentes</t>
   </si>
   <si>
-    <t xml:space="preserve">Conhecendo a comunidade Insper: projetos de software pedagógico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula estúdio para discussão e trabalho em projetos do Insper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pull Requests enviados a projetos da organização Insper no github. </t>
+    <t xml:space="preserve">Introdução a contribuições em projetos abertos - Atividade "Minha primeira contribuição"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula estúdio para atividade em grupo "Minha primeira contribuição"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pull Requests enviados a projetos da externos no Github</t>
   </si>
   <si>
     <t xml:space="preserve">SEMANA DE PROVAS</t>
@@ -257,7 +260,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -271,14 +274,17 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -763,7 +769,7 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -781,7 +787,7 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -793,7 +799,7 @@
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -823,13 +829,13 @@
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -845,7 +851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" ht="76.5">
+    <row r="6" ht="51">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>44439</v>
@@ -863,22 +869,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" ht="102">
+    <row r="7" ht="63.75">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>44441</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
+      <c r="B7" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" ht="13.300000000000001">
@@ -886,17 +892,17 @@
         <f t="shared" si="0"/>
         <v>44446</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>23</v>
+      <c r="B8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" ht="89.25">
@@ -904,17 +910,17 @@
         <f t="shared" si="0"/>
         <v>44448</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" ht="89.25">
@@ -922,53 +928,53 @@
         <f t="shared" si="0"/>
         <v>44453</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>28</v>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" ht="89.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" ht="76.5">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>44455</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>30</v>
+      <c r="B11" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" ht="89.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" ht="63.75">
       <c r="A12" s="3">
         <f t="shared" ref="A12:A34" si="1">A10 + 7</f>
         <v>44460</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>9</v>
@@ -988,17 +994,17 @@
         <f t="shared" si="1"/>
         <v>44462</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="D13" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>9</v>
@@ -1018,17 +1024,17 @@
         <f t="shared" si="1"/>
         <v>44467</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>36</v>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" ht="25.5">
@@ -1036,17 +1042,17 @@
         <f t="shared" si="1"/>
         <v>44469</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>39</v>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" ht="89.25">
@@ -1054,17 +1060,17 @@
         <f t="shared" si="1"/>
         <v>44474</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>39</v>
+      <c r="B16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" ht="51">
@@ -1072,17 +1078,17 @@
         <f t="shared" si="1"/>
         <v>44476</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>36</v>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" ht="25.5">
@@ -1090,17 +1096,17 @@
         <f t="shared" si="1"/>
         <v>44481</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>23</v>
+      <c r="B18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" ht="102">
@@ -1109,16 +1115,16 @@
         <v>44483</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" ht="63.75">
@@ -1127,16 +1133,16 @@
         <v>44488</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" ht="63.75">
@@ -1145,34 +1151,34 @@
         <v>44490</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" ht="63.75">
+      <c r="A22" s="3">
+        <f t="shared" si="1"/>
+        <v>44495</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" ht="102">
-      <c r="A22" s="3">
-        <f t="shared" si="1"/>
-        <v>44495</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" ht="63.75">
@@ -1181,16 +1187,16 @@
         <v>44497</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" ht="51">
@@ -1198,17 +1204,17 @@
         <f t="shared" si="1"/>
         <v>44502</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>23</v>
+      <c r="B24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" ht="63.75">
@@ -1217,16 +1223,16 @@
         <v>44504</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" ht="127.5">
@@ -1235,28 +1241,28 @@
         <v>44509</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="L26" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" ht="63.75">
@@ -1265,16 +1271,16 @@
         <v>44511</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" ht="63.75">
@@ -1283,16 +1289,16 @@
         <v>44516</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" ht="63.75">
@@ -1301,16 +1307,16 @@
         <v>44518</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" ht="102">
@@ -1319,16 +1325,16 @@
         <v>44523</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" ht="102">
@@ -1337,16 +1343,16 @@
         <v>44525</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" ht="63.75">
@@ -1355,16 +1361,16 @@
         <v>44530</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="J32" s="4"/>
     </row>
@@ -1373,17 +1379,17 @@
         <f t="shared" si="1"/>
         <v>44532</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>39</v>
+      <c r="B33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="34" ht="63.75">
@@ -1391,17 +1397,17 @@
         <f t="shared" si="1"/>
         <v>44537</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>39</v>
+      <c r="B34" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="35" ht="63.75">

</xml_diff>

<commit_message>
Atualização aula 09 (que foi movida para 16/09)
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -98,6 +98,9 @@
     <t xml:space="preserve">Expositiva; Atividade prática: reforma de um projeto que apresenta más práticas de projeto</t>
   </si>
   <si>
+    <t>FERIADO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Distribuição e versionamento de software</t>
   </si>
   <si>
@@ -107,9 +110,6 @@
     <t xml:space="preserve">Expositiva; Atividade prática: criação de um pacote Python para distribuição via pip e de um pacote Debian para instalação em sistemas baseados em Debian.</t>
   </si>
   <si>
-    <t>FERIADO</t>
-  </si>
-  <si>
     <t xml:space="preserve">Como fazer software funcionar em vários países?</t>
   </si>
   <si>
@@ -117,6 +117,16 @@
   </si>
   <si>
     <t xml:space="preserve">Expositiva; Atividade prática: tradução e localização de um aplicativo linha de comando e de um sistema web em Flask.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenças de software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direitos autorais no Brasil, patentes e licenças de software;
+Referência: LAURENT Cap 1 e 5, STALLMAN Cap 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expositiva; Atividade prática: discussões de casos relevantes recentes</t>
   </si>
   <si>
     <t xml:space="preserve">Testes de software</t>
@@ -130,16 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">Aula estúdio para atividade “Testes de Software” </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Licenças de software</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direitos autorais no Brasil, patentes e licenças de software;
-Referência: LAURENT Cap 1 e 5, STALLMAN Cap 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expositiva; Atividade prática: discussões de casos relevantes recentes</t>
   </si>
   <si>
     <t xml:space="preserve">Introdução a contribuições em projetos abertos - Atividade "Minha primeira contribuição"</t>
@@ -260,7 +260,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -279,12 +279,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -869,22 +863,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" ht="63.75">
+    <row r="7" ht="89.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>44441</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" ht="13.300000000000001">
@@ -893,70 +887,70 @@
         <v>44446</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" ht="89.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" ht="76.5">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>44448</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" ht="89.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" ht="165.75">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>44453</v>
       </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" ht="76.5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" ht="63.75">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>44455</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>33</v>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" ht="63.75">
@@ -964,17 +958,17 @@
         <f t="shared" ref="A12:A34" si="1">A10 + 7</f>
         <v>44460</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>9</v>
@@ -994,17 +988,17 @@
         <f t="shared" si="1"/>
         <v>44462</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>39</v>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>9</v>
@@ -1024,8 +1018,8 @@
         <f t="shared" si="1"/>
         <v>44467</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>38</v>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>38</v>
@@ -1096,17 +1090,17 @@
         <f t="shared" si="1"/>
         <v>44481</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>26</v>
+      <c r="B18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" ht="102">
@@ -1204,17 +1198,17 @@
         <f t="shared" si="1"/>
         <v>44502</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>26</v>
+      <c r="B24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" ht="63.75">

</xml_diff>

<commit_message>
Change dates in all materials
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -167,10 +167,6 @@
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,7 +679,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -721,7 +717,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="3" s="2" customFormat="1" ht="35.25" customHeight="1">
       <c r="A3" s="4">
         <v>45154</v>
       </c>
@@ -734,9 +730,9 @@
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" s="2" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A4" s="7">
-        <f>A2+7</f>
+    <row r="4" s="2" customFormat="1" ht="57" customHeight="1">
+      <c r="A4" s="4">
+        <f t="shared" ref="A4:A11" si="0">A2+7</f>
         <v>45159</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -749,8 +745,8 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" s="2" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A5" s="7">
-        <f>A3+7</f>
+      <c r="A5" s="4">
+        <f t="shared" si="0"/>
         <v>45161</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -763,8 +759,8 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" s="2" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A6" s="7">
-        <f>A4+7</f>
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
         <v>45166</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -777,8 +773,8 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A7" s="7">
-        <f>A5+7</f>
+      <c r="A7" s="4">
+        <f t="shared" si="0"/>
         <v>45168</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -791,8 +787,8 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8" s="2" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A8" s="7">
-        <f>A6+7</f>
+      <c r="A8" s="4">
+        <f t="shared" si="0"/>
         <v>45173</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -805,8 +801,8 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" s="2" customFormat="1" ht="48" customHeight="1">
-      <c r="A9" s="7">
-        <f>A7+7</f>
+      <c r="A9" s="4">
+        <f t="shared" si="0"/>
         <v>45175</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -819,8 +815,8 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" s="2" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A10" s="7">
-        <f>A8+7</f>
+      <c r="A10" s="4">
+        <f t="shared" si="0"/>
         <v>45180</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -833,8 +829,8 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" s="2" customFormat="1" ht="39" customHeight="1">
-      <c r="A11" s="7">
-        <f>A9+7</f>
+      <c r="A11" s="4">
+        <f t="shared" si="0"/>
         <v>45182</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -847,8 +843,8 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A12" s="7">
-        <f>A10+7</f>
+      <c r="A12" s="4">
+        <f t="shared" ref="A12:A35" si="1">A10+7</f>
         <v>45187</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -861,8 +857,8 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="7">
-        <f>A11+7</f>
+      <c r="A13" s="4">
+        <f t="shared" si="1"/>
         <v>45189</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -875,8 +871,8 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A14" s="7">
-        <f>A12+7</f>
+      <c r="A14" s="4">
+        <f t="shared" si="1"/>
         <v>45194</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -889,8 +885,8 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A15" s="7">
-        <f>A13+7</f>
+      <c r="A15" s="4">
+        <f t="shared" si="1"/>
         <v>45196</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -903,8 +899,8 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A16" s="7">
-        <f>A14+7</f>
+      <c r="A16" s="4">
+        <f t="shared" si="1"/>
         <v>45201</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -917,8 +913,8 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A17" s="7">
-        <f>A15+7</f>
+      <c r="A17" s="4">
+        <f t="shared" si="1"/>
         <v>45203</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -931,8 +927,8 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A18" s="7">
-        <f>A16+7</f>
+      <c r="A18" s="4">
+        <f t="shared" si="1"/>
         <v>45208</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -945,8 +941,8 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A19" s="7">
-        <f>A17+7</f>
+      <c r="A19" s="4">
+        <f t="shared" si="1"/>
         <v>45210</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -959,8 +955,8 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A20" s="7">
-        <f>A18+7</f>
+      <c r="A20" s="4">
+        <f t="shared" si="1"/>
         <v>45215</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -973,8 +969,8 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A21" s="7">
-        <f>A19+7</f>
+      <c r="A21" s="4">
+        <f t="shared" si="1"/>
         <v>45217</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -987,8 +983,8 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A22" s="7">
-        <f>A20+7</f>
+      <c r="A22" s="4">
+        <f t="shared" si="1"/>
         <v>45222</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1001,8 +997,8 @@
       <c r="E22" s="2"/>
     </row>
     <row r="23" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A23" s="7">
-        <f>A21+7</f>
+      <c r="A23" s="4">
+        <f t="shared" si="1"/>
         <v>45224</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1015,8 +1011,8 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A24" s="7">
-        <f>A22+7</f>
+      <c r="A24" s="4">
+        <f t="shared" si="1"/>
         <v>45229</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1029,8 +1025,8 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A25" s="7">
-        <f>A23+7</f>
+      <c r="A25" s="4">
+        <f t="shared" si="1"/>
         <v>45231</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1043,8 +1039,8 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="7">
-        <f>A24+7</f>
+      <c r="A26" s="4">
+        <f t="shared" si="1"/>
         <v>45236</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1057,8 +1053,8 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="7">
-        <f>A25+7</f>
+      <c r="A27" s="4">
+        <f t="shared" si="1"/>
         <v>45238</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1071,8 +1067,8 @@
       <c r="E27" s="2"/>
     </row>
     <row r="28" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="7">
-        <f>A26+7</f>
+      <c r="A28" s="4">
+        <f t="shared" si="1"/>
         <v>45243</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1085,8 +1081,8 @@
       <c r="E28" s="2"/>
     </row>
     <row r="29" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="7">
-        <f>A27+7</f>
+      <c r="A29" s="4">
+        <f t="shared" si="1"/>
         <v>45245</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1099,8 +1095,8 @@
       <c r="E29" s="2"/>
     </row>
     <row r="30" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="7">
-        <f>A28+7</f>
+      <c r="A30" s="4">
+        <f t="shared" si="1"/>
         <v>45250</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -1111,8 +1107,8 @@
       <c r="E30" s="2"/>
     </row>
     <row r="31" s="2" customFormat="1" ht="57">
-      <c r="A31" s="7">
-        <f>A29+7</f>
+      <c r="A31" s="4">
+        <f t="shared" si="1"/>
         <v>45252</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1123,8 +1119,8 @@
       <c r="E31" s="2"/>
     </row>
     <row r="32" s="2" customFormat="1" ht="57">
-      <c r="A32" s="7">
-        <f>A30+7</f>
+      <c r="A32" s="4">
+        <f t="shared" si="1"/>
         <v>45257</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -1135,8 +1131,8 @@
       <c r="E32" s="2"/>
     </row>
     <row r="33" s="2" customFormat="1" ht="57">
-      <c r="A33" s="7">
-        <f>A31+7</f>
+      <c r="A33" s="4">
+        <f t="shared" si="1"/>
         <v>45259</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1147,8 +1143,8 @@
       <c r="E33" s="2"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="57">
-      <c r="A34" s="7">
-        <f>A32+7</f>
+      <c r="A34" s="4">
+        <f t="shared" si="1"/>
         <v>45264</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1161,8 +1157,8 @@
       <c r="E34" s="2"/>
     </row>
     <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A35" s="7">
-        <f>A33+7</f>
+      <c r="A35" s="4">
+        <f t="shared" si="1"/>
         <v>45266</v>
       </c>
       <c r="B35" s="3" t="s">

</xml_diff>

<commit_message>
preparando material versao 2024/2
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -84,6 +84,9 @@
     <t xml:space="preserve">Studio class for group activity "My First Contribution"</t>
   </si>
   <si>
+    <t xml:space="preserve">EXAM WEEK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Working in software communities</t>
   </si>
   <si>
@@ -96,19 +99,19 @@
     <t xml:space="preserve">Studio class for project development</t>
   </si>
   <si>
-    <t xml:space="preserve">EXAM WEEK</t>
+    <t xml:space="preserve">Topics on free culture and software communities</t>
   </si>
   <si>
     <t xml:space="preserve">PUBLIC HOLIDAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Topics on free culture and software communities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="160" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11.000000"/>
@@ -136,17 +139,17 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -167,6 +170,10 @@
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+      <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,7 +713,7 @@
     </row>
     <row r="2" s="2" customFormat="1" ht="41.25" customHeight="1">
       <c r="A2" s="4">
-        <v>45152</v>
+        <v>45518</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -719,7 +726,7 @@
     </row>
     <row r="3" s="2" customFormat="1" ht="35.25" customHeight="1">
       <c r="A3" s="4">
-        <v>45154</v>
+        <v>45523</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -733,7 +740,7 @@
     <row r="4" s="2" customFormat="1" ht="57" customHeight="1">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A11" si="0">A2+7</f>
-        <v>45159</v>
+        <v>45525</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -747,7 +754,7 @@
     <row r="5" s="2" customFormat="1" ht="35.25" customHeight="1">
       <c r="A5" s="4">
         <f t="shared" si="0"/>
-        <v>45161</v>
+        <v>45530</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -761,7 +768,7 @@
     <row r="6" s="2" customFormat="1" ht="44.25" customHeight="1">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
-        <v>45166</v>
+        <v>45532</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -775,7 +782,7 @@
     <row r="7" s="2" customFormat="1" ht="30.75" customHeight="1">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
-        <v>45168</v>
+        <v>45537</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
@@ -789,7 +796,7 @@
     <row r="8" s="2" customFormat="1" ht="36.75" customHeight="1">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
-        <v>45173</v>
+        <v>45539</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>14</v>
@@ -803,7 +810,7 @@
     <row r="9" s="2" customFormat="1" ht="48" customHeight="1">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
-        <v>45175</v>
+        <v>45544</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
@@ -817,7 +824,7 @@
     <row r="10" s="2" customFormat="1" ht="42.75" customHeight="1">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
-        <v>45180</v>
+        <v>45546</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>18</v>
@@ -831,7 +838,7 @@
     <row r="11" s="2" customFormat="1" ht="39" customHeight="1">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
-        <v>45182</v>
+        <v>45551</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
@@ -845,7 +852,7 @@
     <row r="12" s="2" customFormat="1" ht="42.75" customHeight="1">
       <c r="A12" s="4">
         <f t="shared" ref="A12:A35" si="1">A10+7</f>
-        <v>45187</v>
+        <v>45553</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>21</v>
@@ -859,7 +866,7 @@
     <row r="13" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="4">
         <f t="shared" si="1"/>
-        <v>45189</v>
+        <v>45558</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>22</v>
@@ -873,7 +880,7 @@
     <row r="14" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="4">
         <f t="shared" si="1"/>
-        <v>45194</v>
+        <v>45560</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>22</v>
@@ -887,13 +894,13 @@
     <row r="15" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="4">
         <f t="shared" si="1"/>
-        <v>45196</v>
+        <v>45565</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -901,13 +908,13 @@
     <row r="16" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="4">
         <f t="shared" si="1"/>
-        <v>45201</v>
+        <v>45567</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -915,13 +922,13 @@
     <row r="17" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="4">
         <f t="shared" si="1"/>
-        <v>45203</v>
+        <v>45572</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -929,10 +936,10 @@
     <row r="18" s="2" customFormat="1" ht="23.25" customHeight="1">
       <c r="A18" s="4">
         <f t="shared" si="1"/>
-        <v>45208</v>
+        <v>45574</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>27</v>
@@ -943,10 +950,10 @@
     <row r="19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="4">
         <f t="shared" si="1"/>
-        <v>45210</v>
+        <v>45579</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>27</v>
@@ -957,13 +964,13 @@
     <row r="20" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="4">
         <f t="shared" si="1"/>
-        <v>45215</v>
+        <v>45581</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -971,13 +978,13 @@
     <row r="21" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="4">
         <f t="shared" si="1"/>
-        <v>45217</v>
+        <v>45586</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -985,13 +992,13 @@
     <row r="22" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="4">
         <f t="shared" si="1"/>
-        <v>45222</v>
+        <v>45588</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -999,13 +1006,13 @@
     <row r="23" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="4">
         <f t="shared" si="1"/>
-        <v>45224</v>
+        <v>45593</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1013,13 +1020,13 @@
     <row r="24" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="4">
         <f t="shared" si="1"/>
-        <v>45229</v>
+        <v>45595</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1027,13 +1034,13 @@
     <row r="25" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="4">
         <f t="shared" si="1"/>
-        <v>45231</v>
+        <v>45600</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1041,13 +1048,13 @@
     <row r="26" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="4">
         <f t="shared" si="1"/>
-        <v>45236</v>
+        <v>45602</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1055,13 +1062,13 @@
     <row r="27" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="4">
         <f t="shared" si="1"/>
-        <v>45238</v>
+        <v>45607</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1069,13 +1076,13 @@
     <row r="28" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="4">
         <f t="shared" si="1"/>
-        <v>45243</v>
+        <v>45609</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1083,36 +1090,35 @@
     <row r="29" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="4">
         <f t="shared" si="1"/>
-        <v>45245</v>
+        <v>45614</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="4">
         <f t="shared" si="1"/>
-        <v>45250</v>
+        <v>45616</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" s="2" customFormat="1" ht="57">
       <c r="A31" s="4">
         <f t="shared" si="1"/>
-        <v>45252</v>
+        <v>45621</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="2"/>
@@ -1121,10 +1127,10 @@
     <row r="32" s="2" customFormat="1" ht="57">
       <c r="A32" s="4">
         <f t="shared" si="1"/>
-        <v>45257</v>
+        <v>45623</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="2"/>
@@ -1133,25 +1139,27 @@
     <row r="33" s="2" customFormat="1" ht="57">
       <c r="A33" s="4">
         <f t="shared" si="1"/>
-        <v>45259</v>
+        <v>45628</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="57">
       <c r="A34" s="4">
         <f t="shared" si="1"/>
-        <v>45264</v>
+        <v>45630</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1159,21 +1167,28 @@
     <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="4">
         <f t="shared" si="1"/>
-        <v>45266</v>
+        <v>45635</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="A36" s="7">
+        <f>A34+7</f>
+        <v>45637</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>

</xml_diff>

<commit_message>
atualizacao plano de aula
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -24,12 +24,21 @@
     <t>Content</t>
   </si>
   <si>
+    <t>Evidence</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
     <t xml:space="preserve">Introduction to the course and its challenges</t>
   </si>
   <si>
     <t xml:space="preserve">Workflow with distributed version control: forks, patches, pull requests, and local repositories. Technical and non-technical aspects surrounding software: infrastructure, support, marketing, funding. Reference: FOGEL Ch. 3; Additional reading: TAPSCOTT &amp; WILLIAMS.</t>
   </si>
   <si>
+    <t xml:space="preserve">Each completed activity is delivered via a PR in the course repository and serves as evidence for the learning objectives mentioned above.</t>
+  </si>
+  <si>
     <t xml:space="preserve">First code contribution</t>
   </si>
   <si>
@@ -97,6 +106,9 @@
   </si>
   <si>
     <t xml:space="preserve">Studio class for project development</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
   <si>
     <t xml:space="preserve">Topics on free culture and software communities</t>
@@ -109,24 +121,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="160" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11.000000"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8.000000"/>
-      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -161,17 +161,10 @@
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -686,7 +679,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -695,7 +688,8 @@
     <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="14.719285714285713"/>
     <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="53.433571428571433"/>
     <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="54.576428571428572"/>
-    <col bestFit="1" customWidth="1" min="4" max="5" style="2" width="13.005000000000001"/>
+    <col customWidth="1" min="4" max="4" style="2" width="35.28125"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="2" width="13.005000000000001"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -708,487 +702,614 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>45518</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>45523</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="57" customHeight="1">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <f t="shared" ref="A4:A11" si="0">A2+7</f>
         <v>45525</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>45530</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>45532</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>45537</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>45539</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="48" customHeight="1">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>45544</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A10" s="4">
+      <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>45546</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="39" customHeight="1">
-      <c r="A11" s="4">
+      <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>45551</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A12" s="4">
-        <f t="shared" ref="A12:A35" si="1">A10+7</f>
+      <c r="A12" s="5">
+        <f t="shared" ref="A12:A34" si="1">A10+7</f>
         <v>45553</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="4">
+      <c r="A13" s="5">
         <f t="shared" si="1"/>
         <v>45558</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A14" s="4">
+      <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>45560</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A15" s="4">
+      <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>45565</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A16" s="4">
+      <c r="A16" s="5">
         <f t="shared" si="1"/>
         <v>45567</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A17" s="4">
+      <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>45572</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A18" s="4">
+      <c r="A18" s="5">
         <f t="shared" si="1"/>
         <v>45574</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A19" s="4">
+      <c r="A19" s="5">
         <f t="shared" si="1"/>
         <v>45579</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A20" s="4">
+      <c r="A20" s="5">
         <f t="shared" si="1"/>
         <v>45581</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A21" s="4">
+      <c r="A21" s="5">
         <f t="shared" si="1"/>
         <v>45586</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A22" s="4">
+      <c r="A22" s="5">
         <f t="shared" si="1"/>
         <v>45588</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A23" s="4">
+      <c r="A23" s="5">
         <f t="shared" si="1"/>
         <v>45593</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A24" s="4">
+      <c r="A24" s="5">
         <f t="shared" si="1"/>
         <v>45595</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A25" s="4">
+      <c r="A25" s="5">
         <f t="shared" si="1"/>
         <v>45600</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="4">
+      <c r="A26" s="5">
         <f t="shared" si="1"/>
         <v>45602</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="4">
+      <c r="A27" s="5">
         <f t="shared" si="1"/>
         <v>45607</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="4">
+      <c r="A28" s="5">
         <f t="shared" si="1"/>
         <v>45609</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="4">
+      <c r="A29" s="5">
         <f t="shared" si="1"/>
         <v>45614</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="4">
+      <c r="A30" s="5">
         <f t="shared" si="1"/>
         <v>45616</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="E30" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="57">
-      <c r="A31" s="4">
+      <c r="A31" s="5">
         <f t="shared" si="1"/>
         <v>45621</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="57">
-      <c r="A32" s="4">
+      <c r="A32" s="5">
         <f t="shared" si="1"/>
         <v>45623</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="57">
-      <c r="A33" s="4">
+      <c r="A33" s="5">
         <f t="shared" si="1"/>
         <v>45628</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="34" s="2" customFormat="1" ht="57">
-      <c r="A34" s="4">
+      <c r="A34" s="5">
         <f t="shared" si="1"/>
         <v>45630</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
-      <c r="A35" s="4">
-        <f t="shared" si="1"/>
-        <v>45635</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="7">
-        <f>A34+7</f>
-        <v>45637</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>

</xml_diff>